<commit_message>
adjustment of the list number
</commit_message>
<xml_diff>
--- a/labwork4/Чек-лист.xlsx
+++ b/labwork4/Чек-лист.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="193">
   <si>
     <t>N/A</t>
   </si>
@@ -565,6 +565,45 @@
   </si>
   <si>
     <t>2.9</t>
+  </si>
+  <si>
+    <t>1.6.1</t>
+  </si>
+  <si>
+    <t>1.6.2</t>
+  </si>
+  <si>
+    <t>1.6.3</t>
+  </si>
+  <si>
+    <t>1.7.1</t>
+  </si>
+  <si>
+    <t>1.7.2</t>
+  </si>
+  <si>
+    <t>1.7.3</t>
+  </si>
+  <si>
+    <t>1.8.1</t>
+  </si>
+  <si>
+    <t>1.8.2</t>
+  </si>
+  <si>
+    <t>1.8.3</t>
+  </si>
+  <si>
+    <t>1.9.1</t>
+  </si>
+  <si>
+    <t>1.9.2</t>
+  </si>
+  <si>
+    <t>1.9.3</t>
+  </si>
+  <si>
+    <t>2.9.1</t>
   </si>
 </sst>
 </file>
@@ -1204,8 +1243,38 @@
     <xf numFmtId="0" fontId="18" fillId="12" borderId="3" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="3" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="3" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="3" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1214,39 +1283,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1259,10 +1301,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="3" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="3" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="3" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1615,20 +1654,20 @@
       <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:7" ht="23.25">
-      <c r="A2" s="87" t="s">
+      <c r="A2" s="78" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="87"/>
-      <c r="C2" s="87"/>
-      <c r="D2" s="87"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
     </row>
     <row r="3" spans="1:7" ht="45" customHeight="1">
-      <c r="A3" s="89" t="s">
+      <c r="A3" s="80" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="89"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
+      <c r="B3" s="80"/>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
@@ -1637,107 +1676,107 @@
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="88" t="s">
+      <c r="B4" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="88"/>
-      <c r="D4" s="88"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="83" t="s">
+      <c r="B5" s="93" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="81"/>
-      <c r="D5" s="82"/>
+      <c r="C5" s="91"/>
+      <c r="D5" s="92"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="80" t="s">
+      <c r="B6" s="90" t="s">
         <v>56</v>
       </c>
-      <c r="C6" s="81"/>
-      <c r="D6" s="82"/>
+      <c r="C6" s="91"/>
+      <c r="D6" s="92"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="90" t="s">
+      <c r="B7" s="81" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="91"/>
-      <c r="D7" s="92"/>
+      <c r="C7" s="82"/>
+      <c r="D7" s="83"/>
     </row>
     <row r="8" spans="1:7" s="6" customFormat="1" ht="20.25" customHeight="1">
       <c r="A8" s="84" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="93"/>
-      <c r="C8" s="93"/>
-      <c r="D8" s="94"/>
+      <c r="B8" s="85"/>
+      <c r="C8" s="85"/>
+      <c r="D8" s="86"/>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="77" t="s">
+      <c r="B9" s="87" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="78"/>
-      <c r="D9" s="79"/>
+      <c r="C9" s="88"/>
+      <c r="D9" s="89"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="77" t="s">
+      <c r="B10" s="87" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="78"/>
-      <c r="D10" s="79"/>
+      <c r="C10" s="88"/>
+      <c r="D10" s="89"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="77" t="s">
+      <c r="B11" s="87" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="78"/>
-      <c r="D11" s="79"/>
+      <c r="C11" s="88"/>
+      <c r="D11" s="89"/>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="77" t="s">
+      <c r="B12" s="87" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="78"/>
-      <c r="D12" s="79"/>
+      <c r="C12" s="88"/>
+      <c r="D12" s="89"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="77" t="s">
+      <c r="B13" s="87" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="78"/>
-      <c r="D13" s="79"/>
+      <c r="C13" s="88"/>
+      <c r="D13" s="89"/>
     </row>
     <row r="14" spans="1:7" s="9" customFormat="1" ht="22.5" customHeight="1">
       <c r="A14" s="84" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="85"/>
-      <c r="C14" s="85"/>
-      <c r="D14" s="86"/>
+      <c r="B14" s="94"/>
+      <c r="C14" s="94"/>
+      <c r="D14" s="95"/>
     </row>
     <row r="15" spans="1:7" s="9" customFormat="1">
       <c r="A15" s="10" t="s">
@@ -1769,11 +1808,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="A8:D8"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="B5:D5"/>
@@ -1782,6 +1816,11 @@
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="B11:D11"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="A8:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1792,13 +1831,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:J116"/>
+  <dimension ref="A1:J119"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C64" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="F22" sqref="F22"/>
+      <selection pane="bottomRight" activeCell="E106" sqref="E106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -1815,18 +1854,18 @@
         <v>36</v>
       </c>
       <c r="B1" s="29"/>
-      <c r="C1" s="95" t="s">
+      <c r="C1" s="96" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="96"/>
+      <c r="D1" s="97"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="22" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="30"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="99"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="23" t="s">
@@ -2045,7 +2084,7 @@
       <c r="B22" s="52" t="s">
         <v>148</v>
       </c>
-      <c r="C22" s="99" t="s">
+      <c r="C22" s="76" t="s">
         <v>51</v>
       </c>
       <c r="D22" s="25"/>
@@ -2073,7 +2112,9 @@
       <c r="D24" s="44"/>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="36"/>
+      <c r="A25" s="36" t="s">
+        <v>180</v>
+      </c>
       <c r="B25" s="37" t="s">
         <v>176</v>
       </c>
@@ -2084,7 +2125,7 @@
     </row>
     <row r="26" spans="1:4" ht="30">
       <c r="A26" s="36" t="s">
-        <v>81</v>
+        <v>181</v>
       </c>
       <c r="B26" s="37" t="s">
         <v>155</v>
@@ -2096,7 +2137,7 @@
     </row>
     <row r="27" spans="1:4" ht="30">
       <c r="A27" s="36" t="s">
-        <v>82</v>
+        <v>182</v>
       </c>
       <c r="B27" s="37" t="s">
         <v>169</v>
@@ -2117,31 +2158,37 @@
       <c r="D28" s="44"/>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="51"/>
+      <c r="A29" s="51" t="s">
+        <v>183</v>
+      </c>
       <c r="B29" s="52" t="s">
         <v>153</v>
       </c>
-      <c r="C29" s="99" t="s">
+      <c r="C29" s="76" t="s">
         <v>51</v>
       </c>
       <c r="D29" s="25"/>
     </row>
     <row r="30" spans="1:4" ht="30">
-      <c r="A30" s="51"/>
+      <c r="A30" s="51" t="s">
+        <v>184</v>
+      </c>
       <c r="B30" s="52" t="s">
         <v>156</v>
       </c>
-      <c r="C30" s="99" t="s">
+      <c r="C30" s="76" t="s">
         <v>51</v>
       </c>
       <c r="D30" s="25"/>
     </row>
     <row r="31" spans="1:4" ht="30">
-      <c r="A31" s="51"/>
+      <c r="A31" s="51" t="s">
+        <v>185</v>
+      </c>
       <c r="B31" s="52" t="s">
         <v>149</v>
       </c>
-      <c r="C31" s="99" t="s">
+      <c r="C31" s="76" t="s">
         <v>51</v>
       </c>
       <c r="D31" s="25"/>
@@ -2157,31 +2204,37 @@
       <c r="D32" s="44"/>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="51"/>
+      <c r="A33" s="51" t="s">
+        <v>186</v>
+      </c>
       <c r="B33" s="52" t="s">
         <v>153</v>
       </c>
-      <c r="C33" s="99" t="s">
+      <c r="C33" s="76" t="s">
         <v>51</v>
       </c>
       <c r="D33" s="25"/>
     </row>
     <row r="34" spans="1:4" ht="30">
-      <c r="A34" s="51"/>
+      <c r="A34" s="51" t="s">
+        <v>187</v>
+      </c>
       <c r="B34" s="52" t="s">
         <v>156</v>
       </c>
-      <c r="C34" s="99" t="s">
+      <c r="C34" s="76" t="s">
         <v>51</v>
       </c>
       <c r="D34" s="25"/>
     </row>
     <row r="35" spans="1:4" ht="30">
-      <c r="A35" s="51"/>
+      <c r="A35" s="51" t="s">
+        <v>188</v>
+      </c>
       <c r="B35" s="52" t="s">
         <v>149</v>
       </c>
-      <c r="C35" s="99" t="s">
+      <c r="C35" s="76" t="s">
         <v>51</v>
       </c>
       <c r="D35" s="25"/>
@@ -2197,31 +2250,37 @@
       <c r="D36" s="44"/>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="51"/>
+      <c r="A37" s="51" t="s">
+        <v>189</v>
+      </c>
       <c r="B37" s="52" t="s">
         <v>153</v>
       </c>
-      <c r="C37" s="99" t="s">
+      <c r="C37" s="76" t="s">
         <v>51</v>
       </c>
       <c r="D37" s="25"/>
     </row>
     <row r="38" spans="1:4" ht="30">
-      <c r="A38" s="51"/>
+      <c r="A38" s="51" t="s">
+        <v>190</v>
+      </c>
       <c r="B38" s="52" t="s">
         <v>156</v>
       </c>
-      <c r="C38" s="99" t="s">
+      <c r="C38" s="76" t="s">
         <v>51</v>
       </c>
       <c r="D38" s="25"/>
     </row>
     <row r="39" spans="1:4" ht="30">
-      <c r="A39" s="51"/>
+      <c r="A39" s="51" t="s">
+        <v>191</v>
+      </c>
       <c r="B39" s="52" t="s">
         <v>149</v>
       </c>
-      <c r="C39" s="99" t="s">
+      <c r="C39" s="76" t="s">
         <v>51</v>
       </c>
       <c r="D39" s="25"/>
@@ -2425,8 +2484,8 @@
       <c r="B57" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="C57" s="72" t="s">
-        <v>28</v>
+      <c r="C57" s="100" t="s">
+        <v>1</v>
       </c>
       <c r="D57" s="25"/>
     </row>
@@ -2835,7 +2894,9 @@
       <c r="B93" s="49" t="s">
         <v>157</v>
       </c>
-      <c r="C93" s="72"/>
+      <c r="C93" s="72" t="s">
+        <v>28</v>
+      </c>
       <c r="D93" s="25"/>
     </row>
     <row r="94" spans="1:4" ht="30">
@@ -2845,89 +2906,94 @@
       <c r="B94" s="52" t="s">
         <v>160</v>
       </c>
-      <c r="C94" s="72"/>
+      <c r="C94" s="72" t="s">
+        <v>28</v>
+      </c>
       <c r="D94" s="25"/>
     </row>
     <row r="95" spans="1:4">
-      <c r="A95" s="28"/>
-      <c r="B95" s="52"/>
-      <c r="C95" s="72"/>
+      <c r="A95" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="B95" s="52" t="s">
+        <v>161</v>
+      </c>
+      <c r="C95" s="72" t="s">
+        <v>51</v>
+      </c>
       <c r="D95" s="25"/>
     </row>
     <row r="96" spans="1:4">
-      <c r="A96" s="51" t="s">
-        <v>165</v>
-      </c>
-      <c r="B96" s="52" t="s">
-        <v>161</v>
-      </c>
-      <c r="C96" s="76"/>
-      <c r="D96" s="25"/>
+      <c r="A96" s="42" t="s">
+        <v>122</v>
+      </c>
+      <c r="B96" s="53" t="s">
+        <v>109</v>
+      </c>
+      <c r="C96" s="61"/>
+      <c r="D96" s="44"/>
     </row>
     <row r="97" spans="1:10">
-      <c r="A97" s="42" t="s">
-        <v>122</v>
-      </c>
-      <c r="B97" s="53" t="s">
-        <v>109</v>
-      </c>
-      <c r="C97" s="61"/>
-      <c r="D97" s="44"/>
+      <c r="A97" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="B97" s="49" t="s">
+        <v>124</v>
+      </c>
+      <c r="C97" s="72" t="s">
+        <v>51</v>
+      </c>
+      <c r="D97" s="25"/>
     </row>
     <row r="98" spans="1:10">
       <c r="A98" s="28" t="s">
-        <v>123</v>
+        <v>162</v>
       </c>
       <c r="B98" s="49" t="s">
-        <v>124</v>
+        <v>159</v>
       </c>
       <c r="C98" s="72" t="s">
-        <v>51</v>
+        <v>1</v>
       </c>
       <c r="D98" s="25"/>
     </row>
     <row r="99" spans="1:10">
-      <c r="A99" s="28" t="s">
-        <v>162</v>
-      </c>
-      <c r="B99" s="49" t="s">
-        <v>159</v>
-      </c>
-      <c r="C99" s="72"/>
-      <c r="D99" s="25"/>
+      <c r="A99" s="42" t="s">
+        <v>179</v>
+      </c>
+      <c r="B99" s="53" t="s">
+        <v>177</v>
+      </c>
+      <c r="C99" s="77"/>
+      <c r="D99" s="44"/>
     </row>
     <row r="100" spans="1:10">
-      <c r="A100" s="42" t="s">
-        <v>179</v>
-      </c>
-      <c r="B100" s="53" t="s">
-        <v>177</v>
-      </c>
-      <c r="C100" s="100"/>
-      <c r="D100" s="44"/>
+      <c r="A100" s="51" t="s">
+        <v>192</v>
+      </c>
+      <c r="B100" s="52" t="s">
+        <v>178</v>
+      </c>
+      <c r="C100" s="100" t="s">
+        <v>1</v>
+      </c>
+      <c r="D100" s="25"/>
     </row>
     <row r="101" spans="1:10">
-      <c r="A101" s="28"/>
-      <c r="B101" s="49" t="s">
-        <v>178</v>
-      </c>
-      <c r="C101" s="72"/>
-      <c r="D101" s="25"/>
+      <c r="A101"/>
+      <c r="B101"/>
     </row>
     <row r="102" spans="1:10">
       <c r="A102"/>
       <c r="B102"/>
-      <c r="J102" s="35"/>
     </row>
     <row r="103" spans="1:10">
       <c r="A103"/>
       <c r="B103"/>
-      <c r="J103" s="35"/>
     </row>
     <row r="104" spans="1:10">
       <c r="A104"/>
       <c r="B104"/>
-      <c r="J104" s="35"/>
     </row>
     <row r="105" spans="1:10">
       <c r="A105"/>
@@ -2977,12 +3043,22 @@
     <row r="114" spans="1:10">
       <c r="A114"/>
       <c r="B114"/>
+      <c r="J114" s="35"/>
     </row>
     <row r="115" spans="1:10">
-      <c r="F115" s="35"/>
+      <c r="A115"/>
+      <c r="B115"/>
+      <c r="J115" s="35"/>
     </row>
     <row r="116" spans="1:10">
-      <c r="F116" s="35"/>
+      <c r="A116"/>
+      <c r="J116" s="35"/>
+    </row>
+    <row r="118" spans="1:10">
+      <c r="F118" s="35"/>
+    </row>
+    <row r="119" spans="1:10">
+      <c r="F119" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3005,8 +3081,10 @@
     <hyperlink ref="C14" r:id="rId14" display="https://github.com/vliplianina/team2b/issues/76"/>
     <hyperlink ref="C13" r:id="rId15"/>
     <hyperlink ref="C23" r:id="rId16"/>
+    <hyperlink ref="C57" r:id="rId17"/>
+    <hyperlink ref="C100" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId17"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId19"/>
 </worksheet>
 </file>
</xml_diff>